<commit_message>
Better state handling, handshake is now based on initial state of bulb, transmission is considered over when bulb stays on.
</commit_message>
<xml_diff>
--- a/VIPBulbMessageTests.xlsx
+++ b/VIPBulbMessageTests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tombo\Documents\Arduino\VIP-Spring-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09ABBBFC-F6F4-40F2-ACD2-4FFDFF123663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3307AE90-FF69-4EF7-9C9D-1735736421E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCE0195E-F886-4D85-B7CC-CDEEAF9E86A3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>FREQ</t>
   </si>
@@ -92,13 +92,22 @@
   <si>
     <t>Changed message to be much longer</t>
   </si>
+  <si>
+    <t>Improved state machine -&gt; Waits for another handshake after end of transmission and exits handshake if too much time between transitions</t>
+  </si>
+  <si>
+    <t>Reset more variables between transmissions, most importantly "bits"</t>
+  </si>
+  <si>
+    <t>Handshake is now based on initial state of the bulb</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -141,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1979,10 +1988,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D66CB1-F9D8-4E09-8DE4-056EC01FCB75}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,7 +2094,7 @@
         <v>4</v>
       </c>
       <c r="I3" s="3">
-        <f t="shared" ref="I3:I31" si="2">H3/13</f>
+        <f t="shared" ref="I3:I29" si="2">H3/13</f>
         <v>0.30769230769230771</v>
       </c>
       <c r="J3">
@@ -2500,14 +2509,8 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H18" s="2">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="I18" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -2892,6 +2895,219 @@
       </c>
       <c r="J32">
         <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>15</v>
+      </c>
+      <c r="B34">
+        <v>150</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3" t="str">
+        <f t="shared" ref="G34" si="4">IF(F34,E34/F34,"")</f>
+        <v/>
+      </c>
+      <c r="H34" s="2">
+        <f>118-F34</f>
+        <v>118</v>
+      </c>
+      <c r="I34" s="3">
+        <f>H34/118</f>
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>15</v>
+      </c>
+      <c r="B35">
+        <v>150</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <v>12</v>
+      </c>
+      <c r="G35" s="3">
+        <f t="shared" ref="G35:G40" si="5">IF(F35,E35/F35,"")</f>
+        <v>0.5</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" ref="H35:H40" si="6">118-F35</f>
+        <v>106</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" ref="I35:I40" si="7">H35/118</f>
+        <v>0.89830508474576276</v>
+      </c>
+      <c r="J35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>15</v>
+      </c>
+      <c r="B36">
+        <v>150</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <v>12</v>
+      </c>
+      <c r="G36" s="3">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="6"/>
+        <v>106</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="7"/>
+        <v>0.89830508474576276</v>
+      </c>
+      <c r="J36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="H37" s="2"/>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>150</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="6"/>
+        <v>118</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>150</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="6"/>
+        <v>118</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <v>150</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="6"/>
+        <v>118</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New asynchronous encoding scheme. Implemented in TommyEncoding.py, compareTommyBytes.py, and TommyDecoding.ino
</commit_message>
<xml_diff>
--- a/VIPBulbMessageTests.xlsx
+++ b/VIPBulbMessageTests.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tombo\Documents\Arduino\VIP-Spring-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3307AE90-FF69-4EF7-9C9D-1735736421E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62179EC6-5803-4A39-9604-4184EC727EE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCE0195E-F886-4D85-B7CC-CDEEAF9E86A3}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{CCE0195E-F886-4D85-B7CC-CDEEAF9E86A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
   <si>
     <t>FREQ</t>
   </si>
@@ -101,6 +103,78 @@
   <si>
     <t>Handshake is now based on initial state of the bulb</t>
   </si>
+  <si>
+    <t>Bits Sent</t>
+  </si>
+  <si>
+    <t>Bytes sent</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
+  </si>
+  <si>
+    <t>Frequency (Hz)</t>
+  </si>
+  <si>
+    <t>Parity Mode</t>
+  </si>
+  <si>
+    <t>Percent Correct</t>
+  </si>
+  <si>
+    <t>Errors Detected</t>
+  </si>
+  <si>
+    <t>***I CHANGE RGB VALUE FROM (0,10,10) TO (0,5,5)</t>
+  </si>
+  <si>
+    <t>***I CHANGED RGB VALUE FROM (0,10,10) to (0,5,5)</t>
+  </si>
+  <si>
+    <t>did not change RGB</t>
+  </si>
+  <si>
+    <t>I did not change RGB</t>
+  </si>
+  <si>
+    <t>Initial State</t>
+  </si>
+  <si>
+    <t>PARITY_LEN</t>
+  </si>
+  <si>
+    <t>PARITY_MODE</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Switch Parity Mode</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>% Detected</t>
+  </si>
+  <si>
+    <t>Bit Sets Correct</t>
+  </si>
+  <si>
+    <t>Letters Correct</t>
+  </si>
+  <si>
+    <t>% letters</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
 </sst>
 </file>
 
@@ -109,7 +183,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +198,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -133,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -141,16 +228,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1988,27 +2109,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D66CB1-F9D8-4E09-8DE4-056EC01FCB75}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="11" width="8.7109375" customWidth="1"/>
+    <col min="3" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="14" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2018,26 +2139,35 @@
       <c r="C1" t="s">
         <v>8</v>
       </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
       <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -2047,29 +2177,29 @@
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" t="str">
-        <f>IF(F2,E2/F2,"")</f>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="str">
+        <f>IF(I2,H2/I2,"")</f>
         <v/>
       </c>
-      <c r="H2" s="2">
-        <f>13-F2</f>
+      <c r="K2" s="2">
+        <f>13-I2</f>
         <v>13</v>
       </c>
-      <c r="I2" s="3">
-        <f>H2/13</f>
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" s="3">
+        <f>K2/13</f>
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -2079,29 +2209,29 @@
       <c r="C3">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="H3">
         <v>6</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>9</v>
       </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G29" si="0">IF(F3,E3/F3,"")</f>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J29" si="0">IF(I3,H3/I3,"")</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="H3" s="2">
-        <f t="shared" ref="H3:H29" si="1">13-F3</f>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K29" si="1">13-I3</f>
         <v>4</v>
       </c>
-      <c r="I3" s="3">
-        <f t="shared" ref="I3:I29" si="2">H3/13</f>
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L29" si="2">K3/13</f>
         <v>0.30769230769230771</v>
       </c>
-      <c r="J3">
+      <c r="M3">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -2111,29 +2241,29 @@
       <c r="C4">
         <v>10</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3" t="str">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H4" s="2">
+      <c r="K4" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I4" s="3">
+      <c r="L4" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -2143,29 +2273,29 @@
       <c r="C5">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <v>6</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>12</v>
       </c>
-      <c r="G5" s="3">
+      <c r="J5" s="3">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H5" s="2">
+      <c r="K5" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I5" s="3">
+      <c r="L5" s="3">
         <f t="shared" si="2"/>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -2175,29 +2305,29 @@
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <v>2</v>
       </c>
-      <c r="G6" s="3">
+      <c r="J6" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H6" s="2">
+      <c r="K6" s="2">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I6" s="3">
+      <c r="L6" s="3">
         <f t="shared" si="2"/>
         <v>0.84615384615384615</v>
       </c>
-      <c r="J6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -2207,37 +2337,37 @@
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3" t="str">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H7" s="2">
+      <c r="K7" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I7" s="3">
+      <c r="L7" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G8" s="3" t="str">
+      <c r="M7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J8" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>15</v>
       </c>
@@ -2247,29 +2377,29 @@
       <c r="C9">
         <v>10</v>
       </c>
-      <c r="E9">
+      <c r="H9">
         <v>6</v>
       </c>
-      <c r="F9">
+      <c r="I9">
         <v>12</v>
       </c>
-      <c r="G9" s="3">
+      <c r="J9" s="3">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H9" s="2">
+      <c r="K9" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I9" s="3">
+      <c r="L9" s="3">
         <f t="shared" si="2"/>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="J9">
+      <c r="M9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>15</v>
       </c>
@@ -2279,29 +2409,29 @@
       <c r="C10">
         <v>10</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3" t="str">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H10" s="2">
+      <c r="K10" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I10" s="3">
+      <c r="L10" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -2311,29 +2441,29 @@
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3" t="str">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H11" s="2">
+      <c r="K11" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I11" s="3">
+      <c r="L11" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>15</v>
       </c>
@@ -2343,29 +2473,29 @@
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="E12">
+      <c r="H12">
         <v>7</v>
       </c>
-      <c r="F12">
+      <c r="I12">
         <v>12</v>
       </c>
-      <c r="G12" s="3">
+      <c r="J12" s="3">
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="H12" s="2">
+      <c r="K12" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I12" s="3">
+      <c r="L12" s="3">
         <f t="shared" si="2"/>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="J12">
+      <c r="M12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
@@ -2375,40 +2505,40 @@
       <c r="C13">
         <v>10</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="2">
+      <c r="K13" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I13" s="3">
+      <c r="L13" s="3">
         <f t="shared" si="2"/>
         <v>0.92307692307692313</v>
       </c>
-      <c r="J13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="3" t="str">
+      <c r="J14" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -2418,29 +2548,29 @@
       <c r="C15">
         <v>10</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3" t="str">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H15" s="2">
+      <c r="K15" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I15" s="3">
+      <c r="L15" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2450,29 +2580,29 @@
       <c r="C16">
         <v>10</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="2">
+      <c r="K16" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I16" s="3">
+      <c r="L16" s="3">
         <f t="shared" si="2"/>
         <v>0.92307692307692313</v>
       </c>
-      <c r="J16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2482,37 +2612,37 @@
       <c r="C17">
         <v>10</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3" t="str">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H17" s="2">
+      <c r="K17" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I17" s="3">
+      <c r="L17" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G18" s="3" t="str">
+      <c r="M17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J18" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>25</v>
       </c>
@@ -2522,29 +2652,29 @@
       <c r="C19">
         <v>10</v>
       </c>
-      <c r="E19">
+      <c r="H19">
         <v>8</v>
       </c>
-      <c r="F19">
-        <v>10</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19" s="3">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="H19" s="2">
+      <c r="K19" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I19" s="3">
+      <c r="L19" s="3">
         <f t="shared" si="2"/>
         <v>0.23076923076923078</v>
       </c>
-      <c r="J19">
+      <c r="M19">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>25</v>
       </c>
@@ -2554,40 +2684,40 @@
       <c r="C20">
         <v>10</v>
       </c>
-      <c r="E20">
+      <c r="H20">
         <v>7</v>
       </c>
-      <c r="F20">
-        <v>10</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="J20" s="3">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="H20" s="2">
+      <c r="K20" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I20" s="3">
+      <c r="L20" s="3">
         <f t="shared" si="2"/>
         <v>0.23076923076923078</v>
       </c>
-      <c r="J20">
+      <c r="M20">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="3" t="str">
+      <c r="J21" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>25</v>
       </c>
@@ -2597,29 +2727,29 @@
       <c r="C22">
         <v>10</v>
       </c>
-      <c r="E22">
+      <c r="H22">
         <v>5</v>
       </c>
-      <c r="F22">
+      <c r="I22">
         <v>5</v>
       </c>
-      <c r="G22" s="3">
+      <c r="J22" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H22" s="2">
+      <c r="K22" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I22" s="3">
+      <c r="L22" s="3">
         <f t="shared" si="2"/>
         <v>0.61538461538461542</v>
       </c>
-      <c r="J22">
+      <c r="M22">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>25</v>
       </c>
@@ -2629,29 +2759,29 @@
       <c r="C23">
         <v>10</v>
       </c>
-      <c r="E23">
+      <c r="H23">
         <v>2</v>
       </c>
-      <c r="F23">
+      <c r="I23">
         <v>11</v>
       </c>
-      <c r="G23" s="3">
+      <c r="J23" s="3">
         <f t="shared" si="0"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H23" s="2">
+      <c r="K23" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I23" s="3">
+      <c r="L23" s="3">
         <f t="shared" si="2"/>
         <v>0.15384615384615385</v>
       </c>
-      <c r="J23">
+      <c r="M23">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>25</v>
       </c>
@@ -2661,29 +2791,29 @@
       <c r="C24">
         <v>10</v>
       </c>
-      <c r="E24">
+      <c r="H24">
         <v>8</v>
       </c>
-      <c r="F24">
+      <c r="I24">
         <v>11</v>
       </c>
-      <c r="G24" s="3">
+      <c r="J24" s="3">
         <f t="shared" si="0"/>
         <v>0.72727272727272729</v>
       </c>
-      <c r="H24" s="2">
+      <c r="K24" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I24" s="3">
+      <c r="L24" s="3">
         <f t="shared" si="2"/>
         <v>0.15384615384615385</v>
       </c>
-      <c r="J24">
+      <c r="M24">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
@@ -2693,40 +2823,40 @@
       <c r="C25">
         <v>10</v>
       </c>
-      <c r="E25">
+      <c r="H25">
         <v>6</v>
       </c>
-      <c r="F25">
+      <c r="I25">
         <v>9</v>
       </c>
-      <c r="G25" s="3">
+      <c r="J25" s="3">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="H25" s="2">
+      <c r="K25" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I25" s="3">
+      <c r="L25" s="3">
         <f t="shared" si="2"/>
         <v>0.30769230769230771</v>
       </c>
-      <c r="J25">
+      <c r="M25">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="3" t="str">
+      <c r="J26" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="2"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>15</v>
       </c>
@@ -2736,29 +2866,29 @@
       <c r="C27">
         <v>10</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27" s="3" t="str">
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H27" s="2">
+      <c r="K27" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I27" s="3">
+      <c r="L27" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J27">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>15</v>
       </c>
@@ -2768,29 +2898,29 @@
       <c r="C28">
         <v>10</v>
       </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3">
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H28" s="2">
+      <c r="K28" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I28" s="3">
+      <c r="L28" s="3">
         <f t="shared" si="2"/>
         <v>0.92307692307692313</v>
       </c>
-      <c r="J28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15</v>
       </c>
@@ -2800,40 +2930,40 @@
       <c r="C29">
         <v>10</v>
       </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29" s="3" t="str">
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H29" s="2">
+      <c r="K29" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I29" s="3">
+      <c r="L29" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J29">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="3" t="str">
-        <f t="shared" ref="G30:G32" si="3">IF(F30,E30/F30,"")</f>
+      <c r="J30" s="3" t="str">
+        <f t="shared" ref="J30:J32" si="3">IF(I30,H30/I30,"")</f>
         <v/>
       </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="2"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>15</v>
       </c>
@@ -2843,29 +2973,29 @@
       <c r="C31">
         <v>10</v>
       </c>
-      <c r="E31">
+      <c r="H31">
         <v>8</v>
       </c>
-      <c r="F31">
+      <c r="I31">
         <v>8</v>
       </c>
-      <c r="G31" s="3">
+      <c r="J31" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="H31" s="2">
-        <f>118-F31</f>
+      <c r="K31" s="2">
+        <f>118-I31</f>
         <v>110</v>
       </c>
-      <c r="I31" s="3">
-        <f>H31/118</f>
+      <c r="L31" s="3">
+        <f>K31/118</f>
         <v>0.93220338983050843</v>
       </c>
-      <c r="J31">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>15</v>
       </c>
@@ -2875,34 +3005,34 @@
       <c r="C32">
         <v>10</v>
       </c>
-      <c r="E32">
-        <v>3</v>
-      </c>
-      <c r="F32">
-        <v>3</v>
-      </c>
-      <c r="G32" s="3">
+      <c r="H32">
+        <v>3</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="J32" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="H32" s="2">
-        <f>118-F32</f>
+      <c r="K32" s="2">
+        <f>118-I32</f>
         <v>115</v>
       </c>
-      <c r="I32" s="3">
-        <f>H32/118</f>
+      <c r="L32" s="3">
+        <f>K32/118</f>
         <v>0.97457627118644063</v>
       </c>
-      <c r="J32">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>15</v>
       </c>
@@ -2912,29 +3042,29 @@
       <c r="C34">
         <v>10</v>
       </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34" s="3" t="str">
-        <f t="shared" ref="G34" si="4">IF(F34,E34/F34,"")</f>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34" s="3" t="str">
+        <f t="shared" ref="J34" si="4">IF(I34,H34/I34,"")</f>
         <v/>
       </c>
-      <c r="H34" s="2">
-        <f>118-F34</f>
-        <v>118</v>
-      </c>
-      <c r="I34" s="3">
-        <f>H34/118</f>
-        <v>1</v>
-      </c>
-      <c r="J34">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="2">
+        <f>13-I34</f>
+        <v>13</v>
+      </c>
+      <c r="L34" s="3">
+        <f>K34/13</f>
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>15</v>
       </c>
@@ -2944,29 +3074,29 @@
       <c r="C35">
         <v>10</v>
       </c>
-      <c r="E35">
+      <c r="H35">
         <v>6</v>
       </c>
-      <c r="F35">
+      <c r="I35">
         <v>12</v>
       </c>
-      <c r="G35" s="3">
-        <f t="shared" ref="G35:G40" si="5">IF(F35,E35/F35,"")</f>
+      <c r="J35" s="3">
+        <f t="shared" ref="J35:J55" si="5">IF(I35,H35/I35,"")</f>
         <v>0.5</v>
       </c>
-      <c r="H35" s="2">
-        <f t="shared" ref="H35:H40" si="6">118-F35</f>
-        <v>106</v>
-      </c>
-      <c r="I35" s="3">
-        <f t="shared" ref="I35:I40" si="7">H35/118</f>
-        <v>0.89830508474576276</v>
-      </c>
-      <c r="J35">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="2">
+        <f t="shared" ref="K35:K55" si="6">13-I35</f>
+        <v>1</v>
+      </c>
+      <c r="L35" s="3">
+        <f t="shared" ref="L35:L55" si="7">K35/13</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="M35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>15</v>
       </c>
@@ -2976,40 +3106,46 @@
       <c r="C36">
         <v>10</v>
       </c>
-      <c r="E36">
+      <c r="H36">
         <v>4</v>
       </c>
-      <c r="F36">
+      <c r="I36">
         <v>12</v>
       </c>
-      <c r="G36" s="3">
+      <c r="J36" s="3">
         <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="H36" s="2">
+      <c r="K36" s="2">
         <f t="shared" si="6"/>
-        <v>106</v>
-      </c>
-      <c r="I36" s="3">
+        <v>1</v>
+      </c>
+      <c r="L36" s="3">
         <f t="shared" si="7"/>
-        <v>0.89830508474576276</v>
-      </c>
-      <c r="J36">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="M36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
-      <c r="G37" s="3" t="str">
+      <c r="J37" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="2">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="L37" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>15</v>
       </c>
@@ -3019,29 +3155,29 @@
       <c r="C38">
         <v>10</v>
       </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38" s="3" t="str">
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="H38" s="2">
+      <c r="K38" s="2">
         <f t="shared" si="6"/>
-        <v>118</v>
-      </c>
-      <c r="I38" s="3">
+        <v>13</v>
+      </c>
+      <c r="L38" s="3">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="J38">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>15</v>
       </c>
@@ -3051,29 +3187,29 @@
       <c r="C39">
         <v>10</v>
       </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39" s="3" t="str">
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="H39" s="2">
+      <c r="K39" s="2">
         <f t="shared" si="6"/>
-        <v>118</v>
-      </c>
-      <c r="I39" s="3">
+        <v>13</v>
+      </c>
+      <c r="L39" s="3">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="J39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>15</v>
       </c>
@@ -3083,31 +3219,1351 @@
       <c r="C40">
         <v>10</v>
       </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40" s="3" t="str">
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="H40" s="2">
+      <c r="K40" s="2">
         <f t="shared" si="6"/>
-        <v>118</v>
-      </c>
-      <c r="I40" s="3">
+        <v>13</v>
+      </c>
+      <c r="L40" s="3">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="J40">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>21</v>
+      </c>
+      <c r="J41" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K41" s="2"/>
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>150</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K42" s="2">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="L42" s="3">
+        <f t="shared" si="7"/>
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="M42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>15</v>
+      </c>
+      <c r="B43">
+        <v>150</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" t="s">
+        <v>37</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K43" s="2">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="L43" s="3">
+        <f t="shared" si="7"/>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="M43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>15</v>
+      </c>
+      <c r="B44">
+        <v>150</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" t="s">
+        <v>37</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>7</v>
+      </c>
+      <c r="I44">
+        <v>13</v>
+      </c>
+      <c r="J44" s="3">
+        <f t="shared" si="5"/>
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="K44" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L44" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <v>150</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>8</v>
+      </c>
+      <c r="I45">
+        <v>13</v>
+      </c>
+      <c r="J45" s="3">
+        <f t="shared" si="5"/>
+        <v>0.61538461538461542</v>
+      </c>
+      <c r="K45" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L45" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>150</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+      <c r="I46">
+        <v>13</v>
+      </c>
+      <c r="J46" s="3">
+        <f t="shared" si="5"/>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="K46" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L46" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>150</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K47" s="2">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="L47" s="3">
+        <f t="shared" si="7"/>
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="M47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>15</v>
+      </c>
+      <c r="B48">
+        <v>150</v>
+      </c>
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
+      </c>
+      <c r="I48">
+        <v>13</v>
+      </c>
+      <c r="J48" s="3">
+        <f t="shared" si="5"/>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="K48" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L48" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>15</v>
+      </c>
+      <c r="B49">
+        <v>150</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>5</v>
+      </c>
+      <c r="I49">
+        <v>5</v>
+      </c>
+      <c r="J49" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K49" s="2">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="L49" s="3">
+        <f t="shared" si="7"/>
+        <v>0.61538461538461542</v>
+      </c>
+      <c r="M49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>38</v>
+      </c>
+      <c r="J50" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K50" s="2"/>
+      <c r="L50" s="3"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>150</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>36</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K51" s="2">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="L51" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>15</v>
+      </c>
+      <c r="B52">
+        <v>150</v>
+      </c>
+      <c r="C52">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K52" s="2">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="L52" s="3">
+        <f t="shared" si="7"/>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="M52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>15</v>
+      </c>
+      <c r="B53">
+        <v>150</v>
+      </c>
+      <c r="C53">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>2</v>
+      </c>
+      <c r="J53" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="K53" s="2">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="L53" s="3">
+        <f t="shared" si="7"/>
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="M53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>15</v>
+      </c>
+      <c r="B54">
+        <v>150</v>
+      </c>
+      <c r="C54">
+        <v>10</v>
+      </c>
+      <c r="D54" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K54" s="2">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="L54" s="3">
+        <f t="shared" si="7"/>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="M54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>15</v>
+      </c>
+      <c r="B55">
+        <v>150</v>
+      </c>
+      <c r="C55">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>60</v>
+      </c>
+      <c r="I55">
+        <v>16</v>
+      </c>
+      <c r="J55" s="3">
+        <f t="shared" si="5"/>
+        <v>3.75</v>
+      </c>
+      <c r="K55" s="2">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="L55" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.23076923076923078</v>
+      </c>
+      <c r="M55">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B9E57D-1420-4DC2-97FF-B2666E85AC4D}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>72</v>
+      </c>
+      <c r="B2" s="6">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>72</v>
+      </c>
+      <c r="B3" s="6">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.66</v>
+      </c>
+      <c r="G3" s="6">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>72</v>
+      </c>
+      <c r="B5" s="6">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.89</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>248</v>
+      </c>
+      <c r="B7" s="6">
+        <v>31</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>248</v>
+      </c>
+      <c r="B8" s="6">
+        <v>31</v>
+      </c>
+      <c r="C8" s="6">
+        <v>20</v>
+      </c>
+      <c r="D8" s="6">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="G8" s="6">
+        <v>13</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>248</v>
+      </c>
+      <c r="B9" s="6">
+        <v>31</v>
+      </c>
+      <c r="C9" s="6">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.68</v>
+      </c>
+      <c r="G9" s="6">
+        <v>7</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>248</v>
+      </c>
+      <c r="B10" s="6">
+        <v>31</v>
+      </c>
+      <c r="C10" s="6">
+        <v>20</v>
+      </c>
+      <c r="D10" s="6">
+        <v>15</v>
+      </c>
+      <c r="E10" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="G10" s="6">
+        <v>5</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>248</v>
+      </c>
+      <c r="B11" s="6">
+        <v>31</v>
+      </c>
+      <c r="C11" s="6">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6">
+        <v>14</v>
+      </c>
+      <c r="E11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.84</v>
+      </c>
+      <c r="G11" s="6">
+        <v>2</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>280</v>
+      </c>
+      <c r="B13" s="6">
+        <v>35</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6">
+        <v>10</v>
+      </c>
+      <c r="E13" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>280</v>
+      </c>
+      <c r="B14" s="6">
+        <v>35</v>
+      </c>
+      <c r="C14" s="6">
+        <v>4</v>
+      </c>
+      <c r="D14" s="6">
+        <v>15</v>
+      </c>
+      <c r="E14" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.89</v>
+      </c>
+      <c r="G14" s="6">
+        <v>2</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>280</v>
+      </c>
+      <c r="B15" s="6">
+        <v>35</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6">
+        <v>10</v>
+      </c>
+      <c r="E15" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.94</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>280</v>
+      </c>
+      <c r="B16" s="6">
+        <v>35</v>
+      </c>
+      <c r="C16" s="6">
+        <v>13</v>
+      </c>
+      <c r="D16" s="6">
+        <v>15</v>
+      </c>
+      <c r="E16" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.63</v>
+      </c>
+      <c r="G16" s="6">
+        <v>5</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF418E2F-F053-493F-8E73-D70BB579630A}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>150</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f>IF(H2,G2/H2,"")</f>
+        <v/>
+      </c>
+      <c r="J2" s="2">
+        <f>29-H2</f>
+        <v>29</v>
+      </c>
+      <c r="K2" s="3">
+        <f>J2/29</f>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>13</v>
+      </c>
+      <c r="M2" s="10">
+        <f>L2/13</f>
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>150</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="str">
+        <f t="shared" ref="I3:I7" si="0">IF(H3,G3/H3,"")</f>
+        <v/>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J7" si="1">29-H3</f>
+        <v>29</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K9" si="2">J3/29</f>
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>13</v>
+      </c>
+      <c r="M3" s="10">
+        <f t="shared" ref="M3:M9" si="3">L3/13</f>
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="2"/>
+        <v>0.93103448275862066</v>
+      </c>
+      <c r="L4">
+        <v>11</v>
+      </c>
+      <c r="M4" s="10">
+        <f t="shared" si="3"/>
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="N4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>150</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>13</v>
+      </c>
+      <c r="M5" s="10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>150</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>13</v>
+      </c>
+      <c r="M6" s="10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>150</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.96551724137931039</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7" s="10">
+        <f t="shared" si="3"/>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="N7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I8" s="3" t="str">
+        <f t="shared" ref="I8:I9" si="4">IF(H8,G8/H8,"")</f>
+        <v/>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>27</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" ref="J8:J9" si="5">29-H9</f>
+        <v>2</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="2"/>
+        <v>6.8965517241379309E-2</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9" s="10">
+        <f t="shared" si="3"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="N9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>150</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>91</v>
+      </c>
+      <c r="N11">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>